<commit_message>
had meeting with professor Jerman, created ToDos and updated a few Datasheets
</commit_message>
<xml_diff>
--- a/parts-list-printhead.xlsx
+++ b/parts-list-printhead.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://htlkaindorfat-my.sharepoint.com/personal/pla_htl-kaindorf_at/Documents/HTL/4_EL/Wortuhr/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jan\Documents\github\fiberprinter-electronics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1650" documentId="14_{0A081108-4B93-4005-A723-FEF5B27231B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{81764758-725A-1D49-B994-A3E578F0A56F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44248496-3310-4938-9F62-B272295145D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19900" xr2:uid="{AAFC82C3-7438-4009-B0D0-A4268672443D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AAFC82C3-7438-4009-B0D0-A4268672443D}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -1922,13 +1922,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="227">
+  <cellXfs count="222">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
@@ -2141,7 +2143,7 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="75" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2176,7 +2178,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="77" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2244,7 +2246,7 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="82" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2258,78 +2260,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="83" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="83" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -2353,7 +2283,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="90" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="91" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="92" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="93" xfId="0" applyBorder="1"/>
@@ -2361,12 +2290,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="94" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="29" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="95" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="95" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2393,21 +2318,85 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="93" xfId="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="92" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="91" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="91" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
-    <cellStyle name="Link" xfId="2" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2423,9 +2412,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2463,7 +2452,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2569,7 +2558,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2711,7 +2700,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2721,427 +2710,427 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5471192D-BE54-4F16-A81D-71E0167A6568}">
   <dimension ref="A1:AG34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
       <selection pane="bottomLeft" activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
     <col min="3" max="3" width="68" customWidth="1"/>
-    <col min="4" max="4" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="17.5" customWidth="1"/>
-    <col min="12" max="12" width="15.83203125" customWidth="1"/>
+    <col min="10" max="11" width="17.44140625" customWidth="1"/>
+    <col min="12" max="12" width="15.77734375" customWidth="1"/>
     <col min="14" max="14" width="21" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="9.6640625" customWidth="1"/>
     <col min="20" max="20" width="21" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="16.5" customWidth="1"/>
+    <col min="21" max="21" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="16.44140625" customWidth="1"/>
     <col min="26" max="26" width="9.6640625" customWidth="1"/>
     <col min="27" max="27" width="21" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="69" t="s">
+    <row r="1" spans="1:30" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="172" t="s">
+      <c r="B1" s="216" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="173"/>
-      <c r="D1" s="173"/>
-      <c r="E1" s="173"/>
-      <c r="F1" s="173"/>
-      <c r="G1" s="173"/>
-      <c r="H1" s="173"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="6" t="s">
+      <c r="C1" s="217"/>
+      <c r="D1" s="217"/>
+      <c r="E1" s="217"/>
+      <c r="F1" s="217"/>
+      <c r="G1" s="217"/>
+      <c r="H1" s="217"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="71"/>
+      <c r="L1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="160"/>
-      <c r="N1" s="161"/>
-      <c r="O1" s="161"/>
-      <c r="P1" s="161"/>
-      <c r="Q1" s="161"/>
-      <c r="R1" s="6" t="s">
+      <c r="M1" s="204"/>
+      <c r="N1" s="205"/>
+      <c r="O1" s="205"/>
+      <c r="P1" s="205"/>
+      <c r="Q1" s="205"/>
+      <c r="R1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="S1" s="160"/>
-      <c r="T1" s="161"/>
-      <c r="U1" s="161"/>
-      <c r="V1" s="161"/>
-      <c r="W1" s="162"/>
-      <c r="X1" s="6" t="s">
+      <c r="S1" s="204"/>
+      <c r="T1" s="205"/>
+      <c r="U1" s="205"/>
+      <c r="V1" s="205"/>
+      <c r="W1" s="206"/>
+      <c r="X1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="Y1" s="58"/>
-      <c r="Z1" s="160"/>
-      <c r="AA1" s="161"/>
-      <c r="AB1" s="161"/>
-      <c r="AC1" s="161"/>
-      <c r="AD1" s="162"/>
-    </row>
-    <row r="2" spans="1:30" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="166" t="s">
+      <c r="Y1" s="59"/>
+      <c r="Z1" s="204"/>
+      <c r="AA1" s="205"/>
+      <c r="AB1" s="205"/>
+      <c r="AC1" s="205"/>
+      <c r="AD1" s="206"/>
+    </row>
+    <row r="2" spans="1:30" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="210" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="168" t="s">
+      <c r="B2" s="212" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="170" t="s">
+      <c r="C2" s="214" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="168" t="s">
+      <c r="D2" s="212" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="168" t="s">
+      <c r="E2" s="212" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="168" t="s">
+      <c r="F2" s="212" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="168" t="s">
+      <c r="G2" s="212" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="174" t="s">
+      <c r="H2" s="218" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="175" t="s">
+      <c r="I2" s="202" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="178" t="s">
+      <c r="J2" s="200" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="177" t="s">
+      <c r="K2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="164" t="s">
+      <c r="L2" s="208" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="164"/>
-      <c r="N2" s="164"/>
-      <c r="O2" s="164"/>
-      <c r="P2" s="164"/>
-      <c r="Q2" s="165"/>
-      <c r="R2" s="163" t="s">
+      <c r="M2" s="208"/>
+      <c r="N2" s="208"/>
+      <c r="O2" s="208"/>
+      <c r="P2" s="208"/>
+      <c r="Q2" s="209"/>
+      <c r="R2" s="207" t="s">
         <v>16</v>
       </c>
-      <c r="S2" s="164"/>
-      <c r="T2" s="164"/>
-      <c r="U2" s="164"/>
-      <c r="V2" s="164"/>
-      <c r="W2" s="165"/>
-      <c r="X2" s="163" t="s">
+      <c r="S2" s="208"/>
+      <c r="T2" s="208"/>
+      <c r="U2" s="208"/>
+      <c r="V2" s="208"/>
+      <c r="W2" s="209"/>
+      <c r="X2" s="207" t="s">
         <v>17</v>
       </c>
-      <c r="Y2" s="164"/>
-      <c r="Z2" s="164"/>
-      <c r="AA2" s="164"/>
-      <c r="AB2" s="164"/>
-      <c r="AC2" s="164"/>
-      <c r="AD2" s="165"/>
-    </row>
-    <row r="3" spans="1:30" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="167"/>
-      <c r="B3" s="169"/>
-      <c r="C3" s="171"/>
-      <c r="D3" s="169"/>
-      <c r="E3" s="169"/>
-      <c r="F3" s="169"/>
-      <c r="G3" s="169"/>
-      <c r="H3" s="169"/>
-      <c r="I3" s="176"/>
-      <c r="J3" s="179"/>
-      <c r="K3" s="183"/>
-      <c r="L3" s="79" t="s">
+      <c r="Y2" s="208"/>
+      <c r="Z2" s="208"/>
+      <c r="AA2" s="208"/>
+      <c r="AB2" s="208"/>
+      <c r="AC2" s="208"/>
+      <c r="AD2" s="209"/>
+    </row>
+    <row r="3" spans="1:30" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="211"/>
+      <c r="B3" s="213"/>
+      <c r="C3" s="215"/>
+      <c r="D3" s="213"/>
+      <c r="E3" s="213"/>
+      <c r="F3" s="213"/>
+      <c r="G3" s="213"/>
+      <c r="H3" s="213"/>
+      <c r="I3" s="203"/>
+      <c r="J3" s="201"/>
+      <c r="K3" s="199"/>
+      <c r="L3" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="M3" s="75" t="s">
+      <c r="M3" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="N3" s="75" t="s">
+      <c r="N3" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="O3" s="75" t="s">
+      <c r="O3" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="P3" s="75" t="s">
+      <c r="P3" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="Q3" s="80" t="s">
+      <c r="Q3" s="81" t="s">
         <v>23</v>
       </c>
-      <c r="R3" s="74" t="s">
+      <c r="R3" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="S3" s="75" t="s">
+      <c r="S3" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="T3" s="75" t="s">
+      <c r="T3" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="U3" s="75" t="s">
+      <c r="U3" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="V3" s="75" t="s">
+      <c r="V3" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="W3" s="80" t="s">
+      <c r="W3" s="81" t="s">
         <v>23</v>
       </c>
-      <c r="X3" s="193" t="s">
+      <c r="X3" s="170" t="s">
         <v>24</v>
       </c>
-      <c r="Y3" s="194" t="s">
+      <c r="Y3" s="171" t="s">
         <v>18</v>
       </c>
-      <c r="Z3" s="195" t="s">
+      <c r="Z3" s="172" t="s">
         <v>19</v>
       </c>
-      <c r="AA3" s="195" t="s">
+      <c r="AA3" s="172" t="s">
         <v>20</v>
       </c>
-      <c r="AB3" s="195" t="s">
+      <c r="AB3" s="172" t="s">
         <v>21</v>
       </c>
-      <c r="AC3" s="195" t="s">
+      <c r="AC3" s="172" t="s">
         <v>22</v>
       </c>
-      <c r="AD3" s="196" t="s">
+      <c r="AD3" s="173" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:30" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="88"/>
-      <c r="B4" s="89"/>
-      <c r="C4" s="90"/>
-      <c r="D4" s="91"/>
-      <c r="E4" s="89"/>
-      <c r="F4" s="90"/>
-      <c r="G4" s="90"/>
-      <c r="H4" s="92"/>
-      <c r="I4" s="93"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="76"/>
-      <c r="L4" s="223"/>
-      <c r="M4" s="218"/>
-      <c r="N4" s="200"/>
-      <c r="O4" s="219"/>
-      <c r="P4" s="201"/>
-      <c r="Q4" s="202"/>
-      <c r="R4" s="198"/>
-      <c r="S4" s="199"/>
-      <c r="T4" s="200"/>
-      <c r="U4" s="201"/>
-      <c r="V4" s="201"/>
-      <c r="W4" s="202"/>
-      <c r="X4" s="189"/>
-      <c r="Y4" s="189"/>
-      <c r="Z4" s="190"/>
-      <c r="AA4" s="190"/>
-      <c r="AB4" s="191"/>
-      <c r="AC4" s="191"/>
-      <c r="AD4" s="192"/>
-    </row>
-    <row r="5" spans="1:30" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="87"/>
-      <c r="B5" s="94"/>
-      <c r="D5" s="95"/>
-      <c r="E5" s="94"/>
-      <c r="H5" s="96"/>
-      <c r="I5" s="97"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="76"/>
-      <c r="L5" s="224"/>
-      <c r="M5" s="66"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="71"/>
-      <c r="R5" s="203"/>
-      <c r="S5" s="66"/>
-      <c r="T5" s="1"/>
-      <c r="U5" s="2"/>
-      <c r="V5" s="2"/>
-      <c r="W5" s="71"/>
-      <c r="X5" s="59"/>
-      <c r="Y5" s="59"/>
-      <c r="Z5" s="1"/>
-      <c r="AA5" s="1"/>
-      <c r="AB5" s="2"/>
-      <c r="AC5" s="2"/>
-      <c r="AD5" s="159"/>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A6" s="87"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="155"/>
-      <c r="E6" s="156"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="157"/>
-      <c r="I6" s="158"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="76"/>
-      <c r="L6" s="224"/>
-      <c r="M6" s="111"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="71"/>
-      <c r="R6" s="63"/>
-      <c r="S6" s="111"/>
-      <c r="T6" s="1"/>
-      <c r="U6" s="2"/>
-      <c r="V6" s="2"/>
-      <c r="W6" s="71"/>
-      <c r="X6" s="59"/>
-      <c r="Y6" s="59"/>
-      <c r="Z6" s="1"/>
-      <c r="AA6" s="1"/>
-      <c r="AB6" s="2"/>
-      <c r="AC6" s="2"/>
-      <c r="AD6" s="159"/>
-    </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A7" s="87"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="155"/>
-      <c r="E7" s="156"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="157"/>
-      <c r="I7" s="158"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="76"/>
-      <c r="L7" s="224"/>
-      <c r="M7" s="111"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="71"/>
-      <c r="R7" s="30"/>
-      <c r="S7" s="111"/>
-      <c r="T7" s="1"/>
-      <c r="U7" s="2"/>
-      <c r="V7" s="2"/>
-      <c r="W7" s="71"/>
-      <c r="X7" s="59"/>
-      <c r="Y7" s="59"/>
-      <c r="Z7" s="1"/>
-      <c r="AA7" s="1"/>
-      <c r="AB7" s="2"/>
-      <c r="AC7" s="2"/>
-      <c r="AD7" s="159"/>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A8" s="87"/>
-      <c r="D8" s="98"/>
-      <c r="E8" s="94"/>
-      <c r="H8" s="96"/>
-      <c r="I8" s="99"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="214"/>
-      <c r="L8" s="224"/>
-      <c r="M8" s="66"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="71"/>
-      <c r="R8" s="30"/>
-      <c r="S8" s="66"/>
-      <c r="T8" s="1"/>
-      <c r="U8" s="2"/>
-      <c r="V8" s="2"/>
-      <c r="W8" s="71"/>
-      <c r="X8" s="59"/>
-      <c r="Y8" s="59"/>
-      <c r="Z8" s="1"/>
-      <c r="AA8" s="1"/>
-      <c r="AB8" s="2"/>
-      <c r="AC8" s="2"/>
-      <c r="AD8" s="159"/>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A9" s="87"/>
-      <c r="D9" s="98"/>
-      <c r="E9" s="94"/>
-      <c r="H9" s="96"/>
-      <c r="I9" s="99"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="214"/>
-      <c r="L9" s="224"/>
-      <c r="M9" s="66"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="71"/>
-      <c r="R9" s="30"/>
-      <c r="S9" s="66"/>
-      <c r="T9" s="1"/>
-      <c r="U9" s="2"/>
-      <c r="V9" s="2"/>
-      <c r="W9" s="71"/>
-      <c r="X9" s="59"/>
-      <c r="Y9" s="59"/>
-      <c r="Z9" s="1"/>
-      <c r="AA9" s="1"/>
-      <c r="AB9" s="2"/>
-      <c r="AC9" s="2"/>
-      <c r="AD9" s="159"/>
-    </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A10" s="87"/>
-      <c r="D10" s="98"/>
-      <c r="E10" s="94"/>
-      <c r="H10" s="96"/>
-      <c r="I10" s="100"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="214"/>
-      <c r="L10" s="224"/>
-      <c r="M10" s="66"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="71"/>
-      <c r="R10" s="204"/>
-      <c r="S10" s="66"/>
-      <c r="T10" s="1"/>
-      <c r="U10" s="2"/>
-      <c r="V10" s="2"/>
-      <c r="W10" s="71"/>
-      <c r="X10" s="59"/>
-      <c r="Y10" s="59"/>
-      <c r="Z10" s="1"/>
-      <c r="AA10" s="1"/>
-      <c r="AB10" s="2"/>
-      <c r="AC10" s="2"/>
-      <c r="AD10" s="159"/>
-    </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A11" s="87" t="s">
+    <row r="4" spans="1:30" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="89"/>
+      <c r="B4" s="90"/>
+      <c r="C4" s="91"/>
+      <c r="D4" s="92"/>
+      <c r="E4" s="90"/>
+      <c r="F4" s="91"/>
+      <c r="G4" s="91"/>
+      <c r="H4" s="93"/>
+      <c r="I4" s="94"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="77"/>
+      <c r="L4" s="197"/>
+      <c r="M4" s="192"/>
+      <c r="N4" s="176"/>
+      <c r="O4" s="193"/>
+      <c r="P4" s="177"/>
+      <c r="Q4" s="178"/>
+      <c r="R4" s="174"/>
+      <c r="S4" s="175"/>
+      <c r="T4" s="176"/>
+      <c r="U4" s="177"/>
+      <c r="V4" s="177"/>
+      <c r="W4" s="178"/>
+      <c r="X4" s="166"/>
+      <c r="Y4" s="166"/>
+      <c r="Z4" s="167"/>
+      <c r="AA4" s="167"/>
+      <c r="AB4" s="168"/>
+      <c r="AC4" s="168"/>
+      <c r="AD4" s="169"/>
+    </row>
+    <row r="5" spans="1:30" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="88"/>
+      <c r="B5" s="95"/>
+      <c r="D5" s="96"/>
+      <c r="E5" s="95"/>
+      <c r="H5" s="97"/>
+      <c r="I5" s="98"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="77"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="67"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="72"/>
+      <c r="R5" s="179"/>
+      <c r="S5" s="67"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="72"/>
+      <c r="X5" s="60"/>
+      <c r="Y5" s="60"/>
+      <c r="Z5" s="2"/>
+      <c r="AA5" s="2"/>
+      <c r="AB5" s="3"/>
+      <c r="AC5" s="3"/>
+      <c r="AD5" s="160"/>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A6" s="88"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="156"/>
+      <c r="E6" s="157"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="158"/>
+      <c r="I6" s="159"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="77"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="112"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="72"/>
+      <c r="R6" s="64"/>
+      <c r="S6" s="112"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="72"/>
+      <c r="X6" s="60"/>
+      <c r="Y6" s="60"/>
+      <c r="Z6" s="2"/>
+      <c r="AA6" s="2"/>
+      <c r="AB6" s="3"/>
+      <c r="AC6" s="3"/>
+      <c r="AD6" s="160"/>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A7" s="88"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="156"/>
+      <c r="E7" s="157"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="158"/>
+      <c r="I7" s="159"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="77"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="112"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="72"/>
+      <c r="R7" s="31"/>
+      <c r="S7" s="112"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="72"/>
+      <c r="X7" s="60"/>
+      <c r="Y7" s="60"/>
+      <c r="Z7" s="2"/>
+      <c r="AA7" s="2"/>
+      <c r="AB7" s="3"/>
+      <c r="AC7" s="3"/>
+      <c r="AD7" s="160"/>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A8" s="88"/>
+      <c r="D8" s="99"/>
+      <c r="E8" s="95"/>
+      <c r="H8" s="97"/>
+      <c r="I8" s="100"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="188"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="67"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="72"/>
+      <c r="R8" s="31"/>
+      <c r="S8" s="67"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="72"/>
+      <c r="X8" s="60"/>
+      <c r="Y8" s="60"/>
+      <c r="Z8" s="2"/>
+      <c r="AA8" s="2"/>
+      <c r="AB8" s="3"/>
+      <c r="AC8" s="3"/>
+      <c r="AD8" s="160"/>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A9" s="88"/>
+      <c r="D9" s="99"/>
+      <c r="E9" s="95"/>
+      <c r="H9" s="97"/>
+      <c r="I9" s="100"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="188"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="67"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="72"/>
+      <c r="R9" s="31"/>
+      <c r="S9" s="67"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="72"/>
+      <c r="X9" s="60"/>
+      <c r="Y9" s="60"/>
+      <c r="Z9" s="2"/>
+      <c r="AA9" s="2"/>
+      <c r="AB9" s="3"/>
+      <c r="AC9" s="3"/>
+      <c r="AD9" s="160"/>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A10" s="88"/>
+      <c r="D10" s="99"/>
+      <c r="E10" s="95"/>
+      <c r="H10" s="97"/>
+      <c r="I10" s="101"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="188"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="67"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="72"/>
+      <c r="R10" s="180"/>
+      <c r="S10" s="67"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="3"/>
+      <c r="V10" s="3"/>
+      <c r="W10" s="72"/>
+      <c r="X10" s="60"/>
+      <c r="Y10" s="60"/>
+      <c r="Z10" s="2"/>
+      <c r="AA10" s="2"/>
+      <c r="AB10" s="3"/>
+      <c r="AC10" s="3"/>
+      <c r="AD10" s="160"/>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A11" s="88" t="s">
         <v>27</v>
       </c>
       <c r="B11" t="s">
@@ -3150,10 +3139,10 @@
       <c r="C11" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="98" t="s">
+      <c r="D11" s="99" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="94" t="s">
+      <c r="E11" s="95" t="s">
         <v>30</v>
       </c>
       <c r="F11" t="s">
@@ -3162,879 +3151,815 @@
       <c r="G11" t="s">
         <v>32</v>
       </c>
-      <c r="H11" s="96">
+      <c r="H11" s="97">
         <v>1</v>
       </c>
-      <c r="I11" s="99"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="214"/>
-      <c r="L11" s="225"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="4"/>
-      <c r="P11" s="4"/>
-      <c r="Q11" s="220"/>
-      <c r="R11" s="30"/>
-      <c r="S11" s="66"/>
-      <c r="T11" s="1"/>
-      <c r="U11" s="2"/>
-      <c r="V11" s="2"/>
-      <c r="W11" s="71"/>
-      <c r="X11" s="59"/>
-      <c r="Y11" s="59"/>
-      <c r="Z11" s="1"/>
-      <c r="AA11" s="1"/>
-      <c r="AB11" s="2"/>
-      <c r="AC11" s="2"/>
-      <c r="AD11" s="159"/>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A12" s="112" t="s">
+      <c r="I11" s="100"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="188"/>
+      <c r="L11" s="198"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="194"/>
+      <c r="R11" s="31"/>
+      <c r="S11" s="67"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="3"/>
+      <c r="V11" s="3"/>
+      <c r="W11" s="72"/>
+      <c r="X11" s="60"/>
+      <c r="Y11" s="60"/>
+      <c r="Z11" s="2"/>
+      <c r="AA11" s="2"/>
+      <c r="AB11" s="3"/>
+      <c r="AC11" s="3"/>
+      <c r="AD11" s="160"/>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A12" s="113" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="113" t="s">
+      <c r="B12" s="114" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="113" t="s">
+      <c r="C12" s="114" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="117" t="s">
+      <c r="D12" s="118" t="s">
         <v>54</v>
       </c>
-      <c r="E12" s="114" t="s">
+      <c r="E12" s="115" t="s">
         <v>36</v>
       </c>
-      <c r="F12" s="113" t="s">
+      <c r="F12" s="114" t="s">
         <v>37</v>
       </c>
-      <c r="G12" s="113" t="s">
+      <c r="G12" s="114" t="s">
         <v>38</v>
       </c>
-      <c r="H12" s="115">
+      <c r="H12" s="116">
         <v>1</v>
       </c>
-      <c r="I12" s="116"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="214"/>
-      <c r="L12" s="224"/>
-      <c r="M12" s="66"/>
-      <c r="N12" s="205"/>
-      <c r="O12" s="205"/>
-      <c r="P12" s="205"/>
-      <c r="Q12" s="206"/>
-      <c r="R12" s="30"/>
-      <c r="S12" s="205"/>
-      <c r="T12" s="205"/>
-      <c r="U12" s="205"/>
-      <c r="V12" s="205"/>
-      <c r="W12" s="206"/>
-      <c r="X12" s="59"/>
-      <c r="Y12" s="59"/>
-      <c r="Z12" s="1"/>
-      <c r="AA12" s="1"/>
-      <c r="AB12" s="2"/>
-      <c r="AC12" s="2"/>
-      <c r="AD12" s="159"/>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A13" s="106" t="s">
+      <c r="I12" s="117"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="188"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="67"/>
+      <c r="Q12" s="181"/>
+      <c r="R12" s="31"/>
+      <c r="W12" s="181"/>
+      <c r="X12" s="60"/>
+      <c r="Y12" s="60"/>
+      <c r="Z12" s="2"/>
+      <c r="AA12" s="2"/>
+      <c r="AB12" s="3"/>
+      <c r="AC12" s="3"/>
+      <c r="AD12" s="160"/>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A13" s="107" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="101" t="s">
+      <c r="B13" s="102" t="s">
         <v>113</v>
       </c>
-      <c r="C13" s="101" t="s">
+      <c r="C13" s="102" t="s">
         <v>114</v>
       </c>
-      <c r="D13" s="107" t="s">
+      <c r="D13" s="108" t="s">
         <v>54</v>
       </c>
-      <c r="E13" s="103"/>
-      <c r="F13" s="101" t="s">
+      <c r="E13" s="104"/>
+      <c r="F13" s="102" t="s">
         <v>40</v>
       </c>
-      <c r="G13" s="101"/>
-      <c r="H13" s="104">
+      <c r="G13" s="102"/>
+      <c r="H13" s="105">
         <v>1</v>
       </c>
-      <c r="I13" s="123"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="214"/>
-      <c r="L13" s="224"/>
-      <c r="M13" s="66"/>
-      <c r="N13" s="205"/>
-      <c r="O13" s="205"/>
-      <c r="P13" s="205"/>
-      <c r="Q13" s="206"/>
-      <c r="R13" s="30"/>
-      <c r="S13" s="205"/>
-      <c r="T13" s="205"/>
-      <c r="U13" s="205"/>
-      <c r="V13" s="205"/>
-      <c r="W13" s="206"/>
-      <c r="X13" s="59"/>
-      <c r="Y13" s="59"/>
-      <c r="Z13" s="111"/>
-      <c r="AA13" s="1"/>
-      <c r="AB13" s="2"/>
-      <c r="AC13" s="2"/>
-      <c r="AD13" s="159"/>
-    </row>
-    <row r="14" spans="1:30" s="127" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="118" t="s">
+      <c r="I13" s="124"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="188"/>
+      <c r="L13" s="31"/>
+      <c r="M13" s="67"/>
+      <c r="Q13" s="181"/>
+      <c r="R13" s="31"/>
+      <c r="W13" s="181"/>
+      <c r="X13" s="60"/>
+      <c r="Y13" s="60"/>
+      <c r="Z13" s="112"/>
+      <c r="AA13" s="2"/>
+      <c r="AB13" s="3"/>
+      <c r="AC13" s="3"/>
+      <c r="AD13" s="160"/>
+    </row>
+    <row r="14" spans="1:30" s="128" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="119" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="119" t="s">
+      <c r="B14" s="120" t="s">
         <v>117</v>
       </c>
-      <c r="C14" s="120" t="s">
+      <c r="C14" s="121" t="s">
         <v>118</v>
       </c>
-      <c r="D14" s="119"/>
-      <c r="E14" s="110"/>
-      <c r="F14" s="119" t="s">
+      <c r="D14" s="120"/>
+      <c r="E14" s="111"/>
+      <c r="F14" s="120" t="s">
         <v>116</v>
       </c>
-      <c r="G14" s="119" t="s">
+      <c r="G14" s="120" t="s">
         <v>119</v>
       </c>
-      <c r="H14" s="121">
+      <c r="H14" s="122">
         <v>1</v>
       </c>
-      <c r="I14" s="122"/>
-      <c r="J14" s="125"/>
-      <c r="K14" s="215"/>
-      <c r="L14" s="226"/>
-      <c r="M14" s="126"/>
-      <c r="N14" s="208"/>
-      <c r="O14" s="2"/>
-      <c r="P14" s="2"/>
-      <c r="Q14" s="209"/>
-      <c r="R14" s="124"/>
-      <c r="S14" s="207"/>
-      <c r="T14" s="208"/>
-      <c r="U14" s="2"/>
-      <c r="V14" s="2"/>
-      <c r="W14" s="209"/>
-      <c r="X14" s="128"/>
-      <c r="Y14" s="128"/>
-      <c r="Z14" s="26"/>
-      <c r="AA14" s="26"/>
-      <c r="AB14" s="129"/>
-      <c r="AC14" s="129"/>
-      <c r="AD14" s="184"/>
-    </row>
-    <row r="15" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="118" t="s">
+      <c r="I14" s="123"/>
+      <c r="J14" s="126"/>
+      <c r="K14" s="189"/>
+      <c r="L14" s="125"/>
+      <c r="M14" s="127"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="183"/>
+      <c r="R14" s="125"/>
+      <c r="S14" s="182"/>
+      <c r="U14" s="3"/>
+      <c r="V14" s="3"/>
+      <c r="W14" s="183"/>
+      <c r="X14" s="129"/>
+      <c r="Y14" s="129"/>
+      <c r="Z14" s="27"/>
+      <c r="AA14" s="27"/>
+      <c r="AB14" s="130"/>
+      <c r="AC14" s="130"/>
+      <c r="AD14" s="161"/>
+    </row>
+    <row r="15" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="119" t="s">
         <v>142</v>
       </c>
-      <c r="B15" s="119"/>
-      <c r="C15" s="120" t="s">
+      <c r="B15" s="120"/>
+      <c r="C15" s="121" t="s">
         <v>115</v>
       </c>
-      <c r="D15" s="119"/>
-      <c r="E15" s="110"/>
-      <c r="F15" s="119" t="s">
+      <c r="D15" s="120"/>
+      <c r="E15" s="111"/>
+      <c r="F15" s="120" t="s">
         <v>143</v>
       </c>
-      <c r="G15" s="119" t="s">
+      <c r="G15" s="120" t="s">
         <v>144</v>
       </c>
-      <c r="H15" s="121">
+      <c r="H15" s="122">
         <v>1</v>
       </c>
-      <c r="I15" s="122"/>
-      <c r="J15" s="125"/>
-      <c r="K15" s="215"/>
-      <c r="L15" s="224"/>
-      <c r="M15" s="66"/>
-      <c r="N15" s="205"/>
-      <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
-      <c r="Q15" s="206"/>
-      <c r="R15" s="30"/>
-      <c r="S15" s="205"/>
-      <c r="T15" s="205"/>
-      <c r="U15" s="205"/>
-      <c r="V15" s="205"/>
-      <c r="W15" s="206"/>
-      <c r="X15" s="59"/>
-      <c r="Y15" s="59"/>
-      <c r="Z15" s="1"/>
-      <c r="AA15" s="1"/>
-      <c r="AB15" s="2"/>
-      <c r="AC15" s="2"/>
-      <c r="AD15" s="159"/>
-    </row>
-    <row r="16" spans="1:30" s="127" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="118" t="s">
+      <c r="I15" s="123"/>
+      <c r="J15" s="126"/>
+      <c r="K15" s="189"/>
+      <c r="L15" s="31"/>
+      <c r="M15" s="67"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="181"/>
+      <c r="R15" s="31"/>
+      <c r="W15" s="181"/>
+      <c r="X15" s="60"/>
+      <c r="Y15" s="60"/>
+      <c r="Z15" s="2"/>
+      <c r="AA15" s="2"/>
+      <c r="AB15" s="3"/>
+      <c r="AC15" s="3"/>
+      <c r="AD15" s="160"/>
+    </row>
+    <row r="16" spans="1:30" s="128" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="119" t="s">
         <v>120</v>
       </c>
-      <c r="B16" s="119" t="s">
+      <c r="B16" s="120" t="s">
         <v>121</v>
       </c>
-      <c r="C16" s="120" t="s">
+      <c r="C16" s="121" t="s">
         <v>145</v>
       </c>
-      <c r="D16" s="119"/>
-      <c r="E16" s="110" t="s">
+      <c r="D16" s="120"/>
+      <c r="E16" s="111" t="s">
         <v>43</v>
       </c>
-      <c r="F16" s="119" t="s">
+      <c r="F16" s="120" t="s">
         <v>44</v>
       </c>
-      <c r="G16" s="119"/>
-      <c r="H16" s="121">
+      <c r="G16" s="120"/>
+      <c r="H16" s="122">
         <v>0.3</v>
       </c>
-      <c r="I16" s="122"/>
-      <c r="J16" s="125"/>
-      <c r="K16" s="215"/>
-      <c r="L16" s="141"/>
-      <c r="M16" s="133"/>
-      <c r="N16" s="208"/>
-      <c r="O16" s="208"/>
-      <c r="P16" s="208"/>
-      <c r="Q16" s="209"/>
-      <c r="R16" s="141"/>
-      <c r="S16" s="208"/>
-      <c r="T16" s="208"/>
-      <c r="U16" s="208"/>
-      <c r="V16" s="208"/>
-      <c r="W16" s="209"/>
-      <c r="X16" s="128"/>
-      <c r="Y16" s="128"/>
-      <c r="Z16" s="26"/>
-      <c r="AA16" s="26"/>
-      <c r="AB16" s="129"/>
-      <c r="AC16" s="129"/>
-      <c r="AD16" s="184"/>
-    </row>
-    <row r="17" spans="1:33" s="127" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="118" t="s">
+      <c r="I16" s="123"/>
+      <c r="J16" s="126"/>
+      <c r="K16" s="189"/>
+      <c r="L16" s="142"/>
+      <c r="M16" s="134"/>
+      <c r="Q16" s="183"/>
+      <c r="R16" s="142"/>
+      <c r="W16" s="183"/>
+      <c r="X16" s="129"/>
+      <c r="Y16" s="129"/>
+      <c r="Z16" s="27"/>
+      <c r="AA16" s="27"/>
+      <c r="AB16" s="130"/>
+      <c r="AC16" s="130"/>
+      <c r="AD16" s="161"/>
+    </row>
+    <row r="17" spans="1:33" s="128" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="119" t="s">
         <v>122</v>
       </c>
-      <c r="B17" s="119" t="s">
+      <c r="B17" s="120" t="s">
         <v>123</v>
       </c>
-      <c r="C17" s="120" t="s">
+      <c r="C17" s="121" t="s">
         <v>124</v>
       </c>
-      <c r="D17" s="119"/>
-      <c r="E17" s="110"/>
-      <c r="F17" s="119" t="s">
+      <c r="D17" s="120"/>
+      <c r="E17" s="111"/>
+      <c r="F17" s="120" t="s">
         <v>125</v>
       </c>
-      <c r="G17" s="119" t="s">
+      <c r="G17" s="120" t="s">
         <v>126</v>
       </c>
-      <c r="H17" s="121">
+      <c r="H17" s="122">
         <v>3</v>
       </c>
-      <c r="I17" s="122"/>
-      <c r="J17" s="125"/>
-      <c r="K17" s="215"/>
-      <c r="L17" s="124"/>
-      <c r="M17" s="126"/>
-      <c r="N17" s="208"/>
-      <c r="O17" s="2"/>
-      <c r="P17" s="2"/>
-      <c r="Q17" s="209"/>
-      <c r="R17" s="141"/>
-      <c r="S17" s="208"/>
-      <c r="T17" s="208"/>
-      <c r="U17" s="208"/>
-      <c r="V17" s="208"/>
-      <c r="W17" s="209"/>
-      <c r="X17" s="128"/>
-      <c r="Y17" s="128"/>
-      <c r="Z17" s="26"/>
-      <c r="AA17" s="26"/>
-      <c r="AB17" s="129"/>
-      <c r="AC17" s="129"/>
-      <c r="AD17" s="184"/>
-    </row>
-    <row r="18" spans="1:33" s="127" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="118" t="s">
+      <c r="I17" s="123"/>
+      <c r="J17" s="126"/>
+      <c r="K17" s="189"/>
+      <c r="L17" s="125"/>
+      <c r="M17" s="127"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="183"/>
+      <c r="R17" s="142"/>
+      <c r="W17" s="183"/>
+      <c r="X17" s="129"/>
+      <c r="Y17" s="129"/>
+      <c r="Z17" s="27"/>
+      <c r="AA17" s="27"/>
+      <c r="AB17" s="130"/>
+      <c r="AC17" s="130"/>
+      <c r="AD17" s="161"/>
+    </row>
+    <row r="18" spans="1:33" s="128" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="119" t="s">
         <v>128</v>
       </c>
-      <c r="B18" s="119" t="s">
+      <c r="B18" s="120" t="s">
         <v>127</v>
       </c>
-      <c r="C18" s="120" t="s">
+      <c r="C18" s="121" t="s">
         <v>129</v>
       </c>
-      <c r="D18" s="119"/>
-      <c r="E18" s="110" t="s">
+      <c r="D18" s="120"/>
+      <c r="E18" s="111" t="s">
         <v>130</v>
       </c>
-      <c r="F18" s="119" t="s">
+      <c r="F18" s="120" t="s">
         <v>131</v>
       </c>
-      <c r="G18" s="119" t="s">
+      <c r="G18" s="120" t="s">
         <v>45</v>
       </c>
-      <c r="H18" s="121">
+      <c r="H18" s="122">
         <v>8</v>
       </c>
-      <c r="I18" s="122"/>
-      <c r="J18" s="125"/>
-      <c r="K18" s="215"/>
-      <c r="L18" s="124"/>
-      <c r="M18" s="133"/>
-      <c r="N18" s="208"/>
-      <c r="O18" s="2"/>
-      <c r="P18" s="2"/>
-      <c r="Q18" s="209"/>
-      <c r="R18" s="141"/>
-      <c r="S18" s="208"/>
-      <c r="T18" s="208"/>
-      <c r="U18" s="208"/>
-      <c r="V18" s="208"/>
-      <c r="W18" s="209"/>
-      <c r="X18" s="128"/>
-      <c r="Y18" s="128"/>
-      <c r="Z18" s="26"/>
-      <c r="AA18" s="26"/>
-      <c r="AB18" s="129"/>
-      <c r="AC18" s="129"/>
-      <c r="AD18" s="184"/>
-    </row>
-    <row r="19" spans="1:33" s="127" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="118" t="s">
+      <c r="I18" s="123"/>
+      <c r="J18" s="126"/>
+      <c r="K18" s="189"/>
+      <c r="L18" s="125"/>
+      <c r="M18" s="134"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="183"/>
+      <c r="R18" s="142"/>
+      <c r="W18" s="183"/>
+      <c r="X18" s="129"/>
+      <c r="Y18" s="129"/>
+      <c r="Z18" s="27"/>
+      <c r="AA18" s="27"/>
+      <c r="AB18" s="130"/>
+      <c r="AC18" s="130"/>
+      <c r="AD18" s="161"/>
+    </row>
+    <row r="19" spans="1:33" s="128" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="119" t="s">
         <v>132</v>
       </c>
-      <c r="B19" s="119" t="s">
+      <c r="B19" s="120" t="s">
         <v>133</v>
       </c>
-      <c r="C19" s="120" t="s">
+      <c r="C19" s="121" t="s">
         <v>134</v>
       </c>
-      <c r="D19" s="119"/>
-      <c r="E19" s="110" t="s">
+      <c r="D19" s="120"/>
+      <c r="E19" s="111" t="s">
         <v>130</v>
       </c>
-      <c r="F19" s="119" t="s">
+      <c r="F19" s="120" t="s">
         <v>131</v>
       </c>
-      <c r="G19" s="119" t="s">
+      <c r="G19" s="120" t="s">
         <v>46</v>
       </c>
-      <c r="H19" s="121">
+      <c r="H19" s="122">
         <v>4</v>
       </c>
-      <c r="I19" s="122"/>
-      <c r="J19" s="125"/>
-      <c r="K19" s="215"/>
-      <c r="L19" s="124"/>
-      <c r="M19" s="133"/>
-      <c r="N19" s="208"/>
-      <c r="O19" s="129"/>
-      <c r="P19" s="221"/>
-      <c r="Q19" s="209"/>
-      <c r="R19" s="141"/>
-      <c r="S19" s="208"/>
-      <c r="T19" s="208"/>
-      <c r="U19" s="208"/>
-      <c r="V19" s="208"/>
-      <c r="W19" s="209"/>
-      <c r="X19" s="128"/>
-      <c r="Y19" s="128"/>
-      <c r="Z19" s="26"/>
-      <c r="AA19" s="26"/>
-      <c r="AB19" s="129"/>
-      <c r="AC19" s="129"/>
-      <c r="AD19" s="184"/>
-    </row>
-    <row r="20" spans="1:33" s="127" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="118" t="s">
+      <c r="I19" s="123"/>
+      <c r="J19" s="126"/>
+      <c r="K19" s="189"/>
+      <c r="L19" s="125"/>
+      <c r="M19" s="134"/>
+      <c r="O19" s="130"/>
+      <c r="P19" s="195"/>
+      <c r="Q19" s="183"/>
+      <c r="R19" s="142"/>
+      <c r="W19" s="183"/>
+      <c r="X19" s="129"/>
+      <c r="Y19" s="129"/>
+      <c r="Z19" s="27"/>
+      <c r="AA19" s="27"/>
+      <c r="AB19" s="130"/>
+      <c r="AC19" s="130"/>
+      <c r="AD19" s="161"/>
+    </row>
+    <row r="20" spans="1:33" s="128" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="119" t="s">
         <v>135</v>
       </c>
-      <c r="B20" s="119" t="s">
+      <c r="B20" s="120" t="s">
         <v>133</v>
       </c>
-      <c r="C20" s="120" t="s">
+      <c r="C20" s="121" t="s">
         <v>137</v>
       </c>
-      <c r="D20" s="119"/>
-      <c r="E20" s="110" t="s">
+      <c r="D20" s="120"/>
+      <c r="E20" s="111" t="s">
         <v>130</v>
       </c>
-      <c r="F20" s="119" t="s">
+      <c r="F20" s="120" t="s">
         <v>42</v>
       </c>
-      <c r="G20" s="119" t="s">
+      <c r="G20" s="120" t="s">
         <v>47</v>
       </c>
-      <c r="H20" s="121">
+      <c r="H20" s="122">
         <v>3</v>
       </c>
-      <c r="I20" s="122"/>
-      <c r="J20" s="125"/>
-      <c r="K20" s="215"/>
-      <c r="L20" s="124"/>
-      <c r="M20" s="133"/>
-      <c r="N20" s="208"/>
-      <c r="O20" s="129"/>
-      <c r="P20" s="221"/>
-      <c r="Q20" s="209"/>
-      <c r="R20" s="141"/>
-      <c r="S20" s="208"/>
-      <c r="T20" s="208"/>
-      <c r="U20" s="208"/>
-      <c r="V20" s="208"/>
-      <c r="W20" s="209"/>
-      <c r="X20" s="128"/>
-      <c r="Y20" s="128"/>
-      <c r="Z20" s="26"/>
-      <c r="AA20" s="26"/>
-      <c r="AB20" s="129"/>
-      <c r="AC20" s="129"/>
-      <c r="AD20" s="184"/>
-    </row>
-    <row r="21" spans="1:33" s="127" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="118" t="s">
+      <c r="I20" s="123"/>
+      <c r="J20" s="126"/>
+      <c r="K20" s="189"/>
+      <c r="L20" s="125"/>
+      <c r="M20" s="134"/>
+      <c r="O20" s="130"/>
+      <c r="P20" s="195"/>
+      <c r="Q20" s="183"/>
+      <c r="R20" s="142"/>
+      <c r="W20" s="183"/>
+      <c r="X20" s="129"/>
+      <c r="Y20" s="129"/>
+      <c r="Z20" s="27"/>
+      <c r="AA20" s="27"/>
+      <c r="AB20" s="130"/>
+      <c r="AC20" s="130"/>
+      <c r="AD20" s="161"/>
+    </row>
+    <row r="21" spans="1:33" s="128" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="119" t="s">
         <v>136</v>
       </c>
-      <c r="B21" s="119" t="s">
+      <c r="B21" s="120" t="s">
         <v>138</v>
       </c>
-      <c r="C21" s="131" t="s">
+      <c r="C21" s="132" t="s">
         <v>139</v>
       </c>
-      <c r="D21" s="119"/>
-      <c r="E21" s="131"/>
-      <c r="F21" s="119" t="s">
+      <c r="D21" s="120"/>
+      <c r="E21" s="132"/>
+      <c r="F21" s="120" t="s">
         <v>140</v>
       </c>
-      <c r="G21" s="119" t="s">
+      <c r="G21" s="120" t="s">
         <v>141</v>
       </c>
-      <c r="H21" s="121">
+      <c r="H21" s="122">
         <v>1</v>
       </c>
-      <c r="I21" s="122"/>
-      <c r="J21" s="132"/>
-      <c r="K21" s="216"/>
-      <c r="L21" s="124"/>
-      <c r="M21" s="133"/>
-      <c r="N21" s="208"/>
-      <c r="O21" s="129"/>
-      <c r="P21" s="221"/>
-      <c r="Q21" s="209"/>
-      <c r="R21" s="141"/>
-      <c r="S21" s="208"/>
-      <c r="T21" s="208"/>
-      <c r="U21" s="208"/>
-      <c r="V21" s="208"/>
-      <c r="W21" s="209"/>
-      <c r="X21" s="128"/>
-      <c r="Y21" s="128"/>
-      <c r="Z21" s="26"/>
-      <c r="AA21" s="26"/>
-      <c r="AB21" s="129"/>
-      <c r="AC21" s="129"/>
-      <c r="AD21" s="184"/>
-    </row>
-    <row r="22" spans="1:33" s="140" customFormat="1" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="119" t="s">
+      <c r="I21" s="123"/>
+      <c r="J21" s="133"/>
+      <c r="K21" s="190"/>
+      <c r="L21" s="125"/>
+      <c r="M21" s="134"/>
+      <c r="O21" s="130"/>
+      <c r="P21" s="195"/>
+      <c r="Q21" s="183"/>
+      <c r="R21" s="142"/>
+      <c r="W21" s="183"/>
+      <c r="X21" s="129"/>
+      <c r="Y21" s="129"/>
+      <c r="Z21" s="27"/>
+      <c r="AA21" s="27"/>
+      <c r="AB21" s="130"/>
+      <c r="AC21" s="130"/>
+      <c r="AD21" s="161"/>
+    </row>
+    <row r="22" spans="1:33" s="141" customFormat="1" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="120" t="s">
         <v>48</v>
       </c>
-      <c r="B22" s="119"/>
-      <c r="C22" s="131" t="s">
+      <c r="B22" s="120"/>
+      <c r="C22" s="132" t="s">
         <v>146</v>
       </c>
-      <c r="D22" s="134" t="s">
+      <c r="D22" s="135" t="s">
         <v>49</v>
       </c>
-      <c r="E22" s="110"/>
-      <c r="F22" s="119" t="s">
+      <c r="E22" s="111"/>
+      <c r="F22" s="120" t="s">
         <v>50</v>
       </c>
-      <c r="G22" s="119"/>
-      <c r="H22" s="121">
+      <c r="G22" s="120"/>
+      <c r="H22" s="122">
         <v>2.5</v>
       </c>
-      <c r="I22" s="122"/>
-      <c r="J22" s="135"/>
-      <c r="K22" s="217"/>
-      <c r="L22" s="124"/>
-      <c r="M22" s="133"/>
-      <c r="N22" s="136"/>
-      <c r="O22" s="137"/>
-      <c r="P22" s="137"/>
-      <c r="Q22" s="210"/>
-      <c r="R22" s="124"/>
-      <c r="S22" s="138"/>
-      <c r="T22" s="136"/>
-      <c r="U22" s="137"/>
-      <c r="V22" s="137"/>
-      <c r="W22" s="210"/>
-      <c r="X22" s="128"/>
-      <c r="Y22" s="128"/>
-      <c r="Z22" s="26"/>
-      <c r="AA22" s="26"/>
-      <c r="AB22" s="129"/>
-      <c r="AC22" s="129"/>
-      <c r="AD22" s="184"/>
-      <c r="AE22" s="139"/>
-      <c r="AF22" s="139"/>
-      <c r="AG22" s="139"/>
-    </row>
-    <row r="23" spans="1:33" s="127" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="142" t="s">
+      <c r="I22" s="123"/>
+      <c r="J22" s="136"/>
+      <c r="K22" s="191"/>
+      <c r="L22" s="125"/>
+      <c r="M22" s="134"/>
+      <c r="N22" s="137"/>
+      <c r="O22" s="138"/>
+      <c r="P22" s="138"/>
+      <c r="Q22" s="184"/>
+      <c r="R22" s="125"/>
+      <c r="S22" s="139"/>
+      <c r="T22" s="137"/>
+      <c r="U22" s="138"/>
+      <c r="V22" s="138"/>
+      <c r="W22" s="184"/>
+      <c r="X22" s="129"/>
+      <c r="Y22" s="129"/>
+      <c r="Z22" s="27"/>
+      <c r="AA22" s="27"/>
+      <c r="AB22" s="130"/>
+      <c r="AC22" s="130"/>
+      <c r="AD22" s="161"/>
+      <c r="AE22" s="140"/>
+      <c r="AF22" s="140"/>
+      <c r="AG22" s="140"/>
+    </row>
+    <row r="23" spans="1:33" s="128" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="143" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="143" t="s">
+      <c r="B23" s="144" t="s">
         <v>52</v>
       </c>
-      <c r="C23" s="143" t="s">
+      <c r="C23" s="144" t="s">
         <v>53</v>
       </c>
-      <c r="D23" s="144" t="s">
+      <c r="D23" s="145" t="s">
         <v>54</v>
       </c>
-      <c r="E23" s="143" t="s">
+      <c r="E23" s="144" t="s">
         <v>25</v>
       </c>
-      <c r="F23" s="145" t="s">
+      <c r="F23" s="146" t="s">
         <v>55</v>
       </c>
-      <c r="G23" s="146" t="s">
+      <c r="G23" s="147" t="s">
         <v>56</v>
       </c>
-      <c r="H23" s="147">
+      <c r="H23" s="148">
         <v>1</v>
       </c>
-      <c r="I23" s="148"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="77"/>
-      <c r="L23" s="211"/>
-      <c r="M23" s="149"/>
-      <c r="N23" s="150"/>
-      <c r="O23" s="151"/>
-      <c r="P23" s="151"/>
-      <c r="Q23" s="212"/>
-      <c r="R23" s="211"/>
-      <c r="S23" s="150"/>
-      <c r="T23" s="150"/>
-      <c r="U23" s="151"/>
-      <c r="V23" s="151"/>
-      <c r="W23" s="212"/>
-      <c r="X23" s="197"/>
-      <c r="Y23" s="153"/>
-      <c r="Z23" s="154"/>
-      <c r="AA23" s="150"/>
-      <c r="AB23" s="151"/>
-      <c r="AC23" s="151"/>
-      <c r="AD23" s="152"/>
-    </row>
-    <row r="24" spans="1:33" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="106" t="s">
+      <c r="I23" s="149"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="78"/>
+      <c r="L23" s="185"/>
+      <c r="M23" s="150"/>
+      <c r="N23" s="151"/>
+      <c r="O23" s="152"/>
+      <c r="P23" s="152"/>
+      <c r="Q23" s="186"/>
+      <c r="R23" s="185"/>
+      <c r="S23" s="151"/>
+      <c r="T23" s="151"/>
+      <c r="U23" s="152"/>
+      <c r="V23" s="152"/>
+      <c r="W23" s="186"/>
+      <c r="X23" s="154"/>
+      <c r="Y23" s="154"/>
+      <c r="Z23" s="155"/>
+      <c r="AA23" s="151"/>
+      <c r="AB23" s="152"/>
+      <c r="AC23" s="152"/>
+      <c r="AD23" s="153"/>
+    </row>
+    <row r="24" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A24" s="107" t="s">
         <v>57</v>
       </c>
-      <c r="B24" s="101" t="s">
+      <c r="B24" s="102" t="s">
         <v>58</v>
       </c>
-      <c r="C24" s="101" t="s">
+      <c r="C24" s="102" t="s">
         <v>59</v>
       </c>
-      <c r="D24" s="102" t="s">
+      <c r="D24" s="103" t="s">
         <v>54</v>
       </c>
-      <c r="E24" s="107"/>
-      <c r="F24" s="101" t="s">
+      <c r="E24" s="108"/>
+      <c r="F24" s="102" t="s">
         <v>60</v>
       </c>
-      <c r="G24" s="108" t="s">
+      <c r="G24" s="109" t="s">
         <v>61</v>
       </c>
-      <c r="H24" s="104">
+      <c r="H24" s="105">
         <v>0.33</v>
       </c>
-      <c r="I24" s="105"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="214"/>
-      <c r="L24" s="30"/>
-      <c r="M24" s="66"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="2"/>
-      <c r="P24" s="2"/>
-      <c r="Q24" s="71"/>
-      <c r="R24" s="213"/>
-      <c r="S24" s="66"/>
-      <c r="T24" s="1"/>
-      <c r="U24" s="2"/>
-      <c r="V24" s="2"/>
-      <c r="W24" s="71"/>
-      <c r="X24" s="59"/>
-      <c r="Y24" s="59"/>
-      <c r="Z24" s="1"/>
-      <c r="AA24" s="1"/>
-      <c r="AB24" s="2"/>
-      <c r="AC24" s="2"/>
-      <c r="AD24" s="159"/>
-    </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A25" s="106" t="s">
+      <c r="I24" s="106"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="188"/>
+      <c r="L24" s="31"/>
+      <c r="M24" s="67"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="72"/>
+      <c r="R24" s="187"/>
+      <c r="S24" s="67"/>
+      <c r="T24" s="2"/>
+      <c r="U24" s="3"/>
+      <c r="V24" s="3"/>
+      <c r="W24" s="72"/>
+      <c r="X24" s="60"/>
+      <c r="Y24" s="60"/>
+      <c r="Z24" s="2"/>
+      <c r="AA24" s="2"/>
+      <c r="AB24" s="3"/>
+      <c r="AC24" s="3"/>
+      <c r="AD24" s="160"/>
+    </row>
+    <row r="25" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A25" s="107" t="s">
         <v>63</v>
       </c>
-      <c r="B25" s="101" t="s">
+      <c r="B25" s="102" t="s">
         <v>64</v>
       </c>
-      <c r="C25" s="101" t="s">
+      <c r="C25" s="102" t="s">
         <v>65</v>
       </c>
-      <c r="D25" s="102"/>
-      <c r="E25" s="101"/>
-      <c r="F25" s="101" t="s">
+      <c r="D25" s="103"/>
+      <c r="E25" s="102"/>
+      <c r="F25" s="102" t="s">
         <v>66</v>
       </c>
-      <c r="G25" s="110"/>
-      <c r="H25" s="104">
+      <c r="G25" s="111"/>
+      <c r="H25" s="105">
         <v>1</v>
       </c>
-      <c r="I25" s="109"/>
-      <c r="J25" s="12"/>
-      <c r="K25" s="85"/>
-      <c r="L25" s="30"/>
-      <c r="M25" s="66"/>
-      <c r="N25" s="3"/>
-      <c r="O25" s="222"/>
-      <c r="P25" s="4"/>
-      <c r="Q25" s="220"/>
-      <c r="R25" s="213"/>
-      <c r="S25" s="1"/>
-      <c r="T25" s="1"/>
-      <c r="U25" s="2"/>
-      <c r="V25" s="2"/>
-      <c r="W25" s="71"/>
-      <c r="X25" s="60"/>
-      <c r="Y25" s="65"/>
-      <c r="Z25" s="66"/>
-      <c r="AA25" s="1"/>
-      <c r="AB25" s="2"/>
-      <c r="AC25" s="2"/>
-      <c r="AD25" s="159"/>
-    </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A26" s="43" t="s">
+      <c r="I25" s="110"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="86"/>
+      <c r="L25" s="31"/>
+      <c r="M25" s="67"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="196"/>
+      <c r="P25" s="5"/>
+      <c r="Q25" s="194"/>
+      <c r="R25" s="187"/>
+      <c r="S25" s="2"/>
+      <c r="T25" s="2"/>
+      <c r="U25" s="3"/>
+      <c r="V25" s="3"/>
+      <c r="W25" s="72"/>
+      <c r="X25" s="61"/>
+      <c r="Y25" s="66"/>
+      <c r="Z25" s="67"/>
+      <c r="AA25" s="2"/>
+      <c r="AB25" s="3"/>
+      <c r="AC25" s="3"/>
+      <c r="AD25" s="160"/>
+    </row>
+    <row r="26" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A26" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="10"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="11"/>
-      <c r="K26" s="76"/>
-      <c r="L26" s="72"/>
-      <c r="M26" s="9"/>
-      <c r="N26" s="9"/>
-      <c r="O26" s="16"/>
-      <c r="P26" s="16"/>
-      <c r="Q26" s="73"/>
-      <c r="R26" s="72"/>
-      <c r="S26" s="9"/>
-      <c r="T26" s="9"/>
-      <c r="U26" s="16"/>
-      <c r="V26" s="16"/>
-      <c r="W26" s="73"/>
-      <c r="X26" s="61"/>
-      <c r="Y26" s="61"/>
-      <c r="Z26" s="9"/>
-      <c r="AA26" s="9"/>
-      <c r="AB26" s="16"/>
-      <c r="AC26" s="16"/>
-      <c r="AD26" s="185"/>
-    </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A27" s="43" t="s">
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="77"/>
+      <c r="L26" s="73"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="17"/>
+      <c r="P26" s="17"/>
+      <c r="Q26" s="74"/>
+      <c r="R26" s="73"/>
+      <c r="S26" s="10"/>
+      <c r="T26" s="10"/>
+      <c r="U26" s="17"/>
+      <c r="V26" s="17"/>
+      <c r="W26" s="74"/>
+      <c r="X26" s="62"/>
+      <c r="Y26" s="62"/>
+      <c r="Z26" s="10"/>
+      <c r="AA26" s="10"/>
+      <c r="AB26" s="17"/>
+      <c r="AC26" s="17"/>
+      <c r="AD26" s="162"/>
+    </row>
+    <row r="27" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A27" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="C27" s="9"/>
-      <c r="D27" s="15" t="s">
+      <c r="C27" s="10"/>
+      <c r="D27" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9" t="s">
+      <c r="E27" s="10"/>
+      <c r="F27" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="G27" s="9" t="s">
+      <c r="G27" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="H27" s="10">
+      <c r="H27" s="11">
         <v>0.1</v>
       </c>
-      <c r="I27" s="10"/>
-      <c r="J27" s="11"/>
-      <c r="K27" s="76"/>
-      <c r="L27" s="72"/>
-      <c r="M27" s="9"/>
-      <c r="N27" s="9"/>
-      <c r="O27" s="16"/>
-      <c r="P27" s="16"/>
-      <c r="Q27" s="73"/>
-      <c r="R27" s="43"/>
-      <c r="S27" s="18"/>
-      <c r="T27" s="9"/>
-      <c r="U27" s="16"/>
-      <c r="V27" s="16"/>
-      <c r="W27" s="73"/>
-      <c r="X27" s="62"/>
-      <c r="Y27" s="62"/>
-      <c r="Z27" s="18"/>
-      <c r="AA27" s="9"/>
-      <c r="AB27" s="16"/>
-      <c r="AC27" s="16"/>
-      <c r="AD27" s="185"/>
-    </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A28" s="43" t="s">
+      <c r="I27" s="11"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="77"/>
+      <c r="L27" s="73"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="17"/>
+      <c r="P27" s="17"/>
+      <c r="Q27" s="74"/>
+      <c r="R27" s="44"/>
+      <c r="S27" s="19"/>
+      <c r="T27" s="10"/>
+      <c r="U27" s="17"/>
+      <c r="V27" s="17"/>
+      <c r="W27" s="74"/>
+      <c r="X27" s="63"/>
+      <c r="Y27" s="63"/>
+      <c r="Z27" s="19"/>
+      <c r="AA27" s="10"/>
+      <c r="AB27" s="17"/>
+      <c r="AC27" s="17"/>
+      <c r="AD27" s="162"/>
+    </row>
+    <row r="28" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A28" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="C28" s="83"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9" t="s">
+      <c r="C28" s="84"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="G28" s="9" t="s">
+      <c r="G28" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="H28" s="10">
+      <c r="H28" s="11">
         <v>0.1</v>
       </c>
-      <c r="I28" s="10"/>
-      <c r="J28" s="11"/>
-      <c r="K28" s="76"/>
-      <c r="L28" s="43"/>
-      <c r="M28" s="9"/>
-      <c r="N28" s="9"/>
-      <c r="O28" s="16"/>
-      <c r="P28" s="16"/>
-      <c r="Q28" s="73"/>
-      <c r="R28" s="43"/>
-      <c r="S28" s="9"/>
-      <c r="T28" s="9"/>
-      <c r="U28" s="16"/>
-      <c r="V28" s="16"/>
-      <c r="W28" s="73"/>
-      <c r="X28" s="62"/>
-      <c r="Y28" s="62"/>
-      <c r="Z28" s="9"/>
-      <c r="AA28" s="9"/>
-      <c r="AB28" s="16"/>
-      <c r="AC28" s="16"/>
-      <c r="AD28" s="185"/>
-    </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A29" s="43" t="s">
+      <c r="I28" s="11"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="77"/>
+      <c r="L28" s="44"/>
+      <c r="M28" s="10"/>
+      <c r="N28" s="10"/>
+      <c r="O28" s="17"/>
+      <c r="P28" s="17"/>
+      <c r="Q28" s="74"/>
+      <c r="R28" s="44"/>
+      <c r="S28" s="10"/>
+      <c r="T28" s="10"/>
+      <c r="U28" s="17"/>
+      <c r="V28" s="17"/>
+      <c r="W28" s="74"/>
+      <c r="X28" s="63"/>
+      <c r="Y28" s="63"/>
+      <c r="Z28" s="10"/>
+      <c r="AA28" s="10"/>
+      <c r="AB28" s="17"/>
+      <c r="AC28" s="17"/>
+      <c r="AD28" s="162"/>
+    </row>
+    <row r="29" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A29" s="44" t="s">
         <v>80</v>
       </c>
-      <c r="B29" s="17" t="s">
+      <c r="B29" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="C29" s="81"/>
-      <c r="D29" s="82"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9" t="s">
+      <c r="C29" s="82"/>
+      <c r="D29" s="83"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="G29" s="9" t="s">
+      <c r="G29" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="H29" s="10">
+      <c r="H29" s="11">
         <v>0.1</v>
       </c>
-      <c r="I29" s="10"/>
-      <c r="J29" s="11"/>
-      <c r="K29" s="76"/>
-      <c r="L29" s="43"/>
-      <c r="M29" s="9"/>
-      <c r="N29" s="9"/>
-      <c r="O29" s="16"/>
-      <c r="P29" s="16"/>
-      <c r="Q29" s="73"/>
-      <c r="R29" s="43"/>
-      <c r="S29" s="9"/>
-      <c r="T29" s="9"/>
-      <c r="U29" s="16"/>
-      <c r="V29" s="16"/>
-      <c r="W29" s="73"/>
-      <c r="X29" s="62"/>
-      <c r="Y29" s="62"/>
-      <c r="Z29" s="9"/>
-      <c r="AA29" s="9"/>
-      <c r="AB29" s="16"/>
-      <c r="AC29" s="16"/>
-      <c r="AD29" s="185"/>
-    </row>
-    <row r="30" spans="1:33" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="45"/>
-      <c r="B30" s="46"/>
-      <c r="C30" s="84"/>
-      <c r="D30" s="67"/>
-      <c r="E30" s="46"/>
-      <c r="F30" s="46"/>
-      <c r="G30" s="46"/>
-      <c r="H30" s="46"/>
-      <c r="I30" s="46"/>
-      <c r="J30" s="68"/>
-      <c r="K30" s="78"/>
-      <c r="L30" s="45"/>
-      <c r="M30" s="46"/>
-      <c r="N30" s="46"/>
-      <c r="O30" s="46"/>
-      <c r="P30" s="46"/>
-      <c r="Q30" s="47"/>
-      <c r="R30" s="45"/>
-      <c r="S30" s="46"/>
-      <c r="T30" s="46"/>
-      <c r="U30" s="46"/>
-      <c r="V30" s="46"/>
-      <c r="W30" s="47"/>
-      <c r="X30" s="186"/>
-      <c r="Y30" s="186"/>
-      <c r="Z30" s="187"/>
-      <c r="AA30" s="187"/>
-      <c r="AB30" s="187"/>
-      <c r="AC30" s="187"/>
-      <c r="AD30" s="188"/>
-    </row>
-    <row r="32" spans="1:33" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="1:2" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="86" t="s">
+      <c r="I29" s="11"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="77"/>
+      <c r="L29" s="44"/>
+      <c r="M29" s="10"/>
+      <c r="N29" s="10"/>
+      <c r="O29" s="17"/>
+      <c r="P29" s="17"/>
+      <c r="Q29" s="74"/>
+      <c r="R29" s="44"/>
+      <c r="S29" s="10"/>
+      <c r="T29" s="10"/>
+      <c r="U29" s="17"/>
+      <c r="V29" s="17"/>
+      <c r="W29" s="74"/>
+      <c r="X29" s="63"/>
+      <c r="Y29" s="63"/>
+      <c r="Z29" s="10"/>
+      <c r="AA29" s="10"/>
+      <c r="AB29" s="17"/>
+      <c r="AC29" s="17"/>
+      <c r="AD29" s="162"/>
+    </row>
+    <row r="30" spans="1:33" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="46"/>
+      <c r="B30" s="47"/>
+      <c r="C30" s="85"/>
+      <c r="D30" s="68"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="47"/>
+      <c r="J30" s="69"/>
+      <c r="K30" s="79"/>
+      <c r="L30" s="46"/>
+      <c r="M30" s="47"/>
+      <c r="N30" s="47"/>
+      <c r="O30" s="47"/>
+      <c r="P30" s="47"/>
+      <c r="Q30" s="48"/>
+      <c r="R30" s="46"/>
+      <c r="S30" s="47"/>
+      <c r="T30" s="47"/>
+      <c r="U30" s="47"/>
+      <c r="V30" s="47"/>
+      <c r="W30" s="48"/>
+      <c r="X30" s="163"/>
+      <c r="Y30" s="163"/>
+      <c r="Z30" s="164"/>
+      <c r="AA30" s="164"/>
+      <c r="AB30" s="164"/>
+      <c r="AC30" s="164"/>
+      <c r="AD30" s="165"/>
+    </row>
+    <row r="32" spans="1:33" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="33" spans="1:2" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="87" t="s">
         <v>84</v>
       </c>
-      <c r="B33" s="130">
+      <c r="B33" s="131">
         <f>SUM(K4:K30)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="34" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="Z1:AD1"/>
-    <mergeCell ref="X2:AD2"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="C2:C3"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="M1:Q1"/>
     <mergeCell ref="S1:W1"/>
@@ -4042,6 +3967,17 @@
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="L2:Q2"/>
     <mergeCell ref="R2:W2"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="Z1:AD1"/>
+    <mergeCell ref="X2:AD2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F14" r:id="rId1" display="https://at.rs-online.com/web/b/xp-power/" xr:uid="{893D64CB-CE07-4F44-95EF-6DE8A985221B}"/>
@@ -4062,339 +3998,339 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.6640625" customWidth="1"/>
-    <col min="4" max="4" width="32.83203125" customWidth="1"/>
-    <col min="5" max="5" width="66.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.77734375" customWidth="1"/>
+    <col min="5" max="5" width="66.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="48" t="s">
+    <row r="1" spans="1:5" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="180" t="s">
+      <c r="B1" s="219" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="181"/>
-      <c r="D1" s="181"/>
-      <c r="E1" s="182"/>
-    </row>
-    <row r="2" spans="1:5" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
+      <c r="C1" s="220"/>
+      <c r="D1" s="220"/>
+      <c r="E1" s="221"/>
+    </row>
+    <row r="2" spans="1:5" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="50" t="s">
         <v>85</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="29" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="50" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="51" t="s">
         <v>89</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="E3" s="64" t="s">
+      <c r="E3" s="65" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="14" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="31" t="s">
         <v>95</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E4" s="31" t="s">
+      <c r="E4" s="32" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="14" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E5" s="31" t="s">
+      <c r="E5" s="32" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="51" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="52" t="s">
         <v>99</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="D6" s="26" t="s">
+      <c r="D6" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="E6" s="33" t="s">
+      <c r="E6" s="34" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="51" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="32"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="26" t="s">
+      <c r="B7" s="33"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="27" t="s">
         <v>149</v>
       </c>
-      <c r="E7" s="33" t="s">
+      <c r="E7" s="34" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="14" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="31" t="s">
+      <c r="B8" s="31"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="32" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="14"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="31"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="14"/>
-      <c r="B10" s="30"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="31"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="14"/>
-      <c r="B11" s="30"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="31"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="14"/>
-      <c r="B12" s="30"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="31"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="14"/>
-      <c r="B13" s="30"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="31"/>
-    </row>
-    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="14"/>
-      <c r="B14" s="63" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="15"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="32"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="15"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="32"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="15"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="32"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="15"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="32"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="15"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="32"/>
+    </row>
+    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="15"/>
+      <c r="B14" s="64" t="s">
         <v>108</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="31"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="14"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="31"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="14"/>
-      <c r="B16" s="30"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="31"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="14"/>
-      <c r="B17" s="30"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="31"/>
-    </row>
-    <row r="18" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="52"/>
-      <c r="B18" s="34"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="35"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="53" t="s">
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="32"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="15"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="32"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="15"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="32"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="15"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="32"/>
+    </row>
+    <row r="18" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="53"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="36"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="54" t="s">
         <v>57</v>
       </c>
-      <c r="B19" s="36"/>
-      <c r="C19" s="5" t="s">
+      <c r="B19" s="37"/>
+      <c r="C19" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="E19" s="37" t="s">
+      <c r="E19" s="38" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="53" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="B20" s="36"/>
-      <c r="C20" s="5" t="s">
+      <c r="B20" s="37"/>
+      <c r="C20" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="D20" s="5"/>
-      <c r="E20" s="38"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="54" t="s">
+      <c r="D20" s="6"/>
+      <c r="E20" s="39"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="55" t="s">
         <v>63</v>
       </c>
-      <c r="B21" s="39"/>
-      <c r="C21" s="7" t="s">
+      <c r="B21" s="40"/>
+      <c r="C21" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="D21" s="7"/>
-      <c r="E21" s="40" t="s">
+      <c r="D21" s="8"/>
+      <c r="E21" s="41" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="54" t="s">
+    <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="55" t="s">
         <v>111</v>
       </c>
-      <c r="B22" s="39"/>
-      <c r="C22" s="7" t="s">
+      <c r="B22" s="40"/>
+      <c r="C22" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="D22" s="7"/>
-      <c r="E22" s="40" t="s">
+      <c r="D22" s="8"/>
+      <c r="E22" s="41" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="55" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="56" t="s">
         <v>67</v>
       </c>
-      <c r="B23" s="41"/>
-      <c r="C23" s="8" t="s">
+      <c r="B23" s="42"/>
+      <c r="C23" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="D23" s="8"/>
-      <c r="E23" s="42" t="s">
+      <c r="D23" s="9"/>
+      <c r="E23" s="43" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="56" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="57" t="s">
         <v>69</v>
       </c>
-      <c r="B24" s="43"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="44" t="s">
+      <c r="B24" s="44"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="45" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="56" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="57" t="s">
         <v>70</v>
       </c>
-      <c r="B25" s="43"/>
-      <c r="C25" s="9" t="s">
+      <c r="B25" s="44"/>
+      <c r="C25" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="D25" s="9"/>
-      <c r="E25" s="44" t="s">
+      <c r="D25" s="10"/>
+      <c r="E25" s="45" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="56" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="57" t="s">
         <v>72</v>
       </c>
-      <c r="B26" s="43"/>
-      <c r="C26" s="9" t="s">
+      <c r="B26" s="44"/>
+      <c r="C26" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="D26" s="9"/>
-      <c r="E26" s="44" t="s">
+      <c r="D26" s="10"/>
+      <c r="E26" s="45" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="56" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="57" t="s">
         <v>76</v>
       </c>
-      <c r="B27" s="43"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="44" t="s">
+      <c r="B27" s="44"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="45" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="56" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="57" t="s">
         <v>80</v>
       </c>
-      <c r="B28" s="43"/>
-      <c r="C28" s="9" t="s">
+      <c r="B28" s="44"/>
+      <c r="C28" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="D28" s="9"/>
-      <c r="E28" s="44" t="s">
+      <c r="D28" s="10"/>
+      <c r="E28" s="45" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="57"/>
-      <c r="B29" s="45"/>
-      <c r="C29" s="46"/>
-      <c r="D29" s="46"/>
-      <c r="E29" s="47"/>
+    <row r="29" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="58"/>
+      <c r="B29" s="46"/>
+      <c r="C29" s="47"/>
+      <c r="D29" s="47"/>
+      <c r="E29" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4406,6 +4342,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E1477F1D7C7FF24D94CB937C04A5454E" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c5e26cd62d53055273b037171bef2839">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="31d5eec3c12ee2e8127422d567928fa7">
     <xsd:element name="properties">
@@ -4519,34 +4470,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A64FC3A0-F052-4C82-85D7-2707CFD1761B}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A13DC3B0-AB8B-4D41-A874-DE7828CFCA0C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8D8B912-B0EB-4E19-A56B-532404D3CA55}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -4560,4 +4484,28 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A13DC3B0-AB8B-4D41-A874-DE7828CFCA0C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A64FC3A0-F052-4C82-85D7-2707CFD1761B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>